<commit_message>
Initial auto csr_regfile generation
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/csr_spec.xlsx
+++ b/docs/spreadsheets/csr_spec.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">CSR NAME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">CSR_NAME</t>
   </si>
   <si>
     <t xml:space="preserve">ADDRESS</t>
@@ -31,10 +31,13 @@
     <t xml:space="preserve">PRIVILEGE</t>
   </si>
   <si>
-    <t xml:space="preserve">ACCESS (R/W)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESET VALUE</t>
+    <t xml:space="preserve">ACCESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET_VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEHAV</t>
   </si>
   <si>
     <t xml:space="preserve">DESCRIPTION</t>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">R/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">special</t>
   </si>
   <si>
     <t xml:space="preserve">Bottom 32-bits storing number of cycles</t>
@@ -94,6 +100,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -179,16 +186,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="A6:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.89"/>
   </cols>
   <sheetData>
@@ -211,85 +218,100 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>13</v>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
csr implementation and testing complete
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/csr_spec.xlsx
+++ b/docs/spreadsheets/csr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t xml:space="preserve">CSR_NAME</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t xml:space="preserve">Top 32-bits storing number of instructions retired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mstatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">machine status register (currently only used for testing)</t>
   </si>
 </sst>
 </file>
@@ -186,13 +198,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="A6:G7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
@@ -312,6 +324,29 @@
       </c>
       <c r="G5" s="1" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reworked standard system pass condition
</commit_message>
<xml_diff>
--- a/docs/spreadsheets/csr_spec.xlsx
+++ b/docs/spreadsheets/csr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t xml:space="preserve">CSR_NAME</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t xml:space="preserve">machine status register (currently only used for testing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mtest_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7C0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom Register for handelling test success/failure in simulation</t>
   </si>
 </sst>
 </file>
@@ -198,13 +207,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.43"/>
@@ -347,6 +356,29 @@
       </c>
       <c r="G6" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>